<commit_message>
Search user using username
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="37">
   <si>
     <t/>
   </si>
@@ -106,6 +106,24 @@
   </si>
   <si>
     <t>//*[@id="oxd-toaster_1"]/div/div[1]/div[2]/p[2]</t>
+  </si>
+  <si>
+    <t>UM_searchUsername</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/div[2]/div[2]/div/div[1]/div[2]/form/div[1]/div/div[1]/div/div[2]/input</t>
+  </si>
+  <si>
+    <t>UM_searchButton</t>
+  </si>
+  <si>
+    <t>(//button[normalize-space()='Search'])</t>
+  </si>
+  <si>
+    <t>UM_searchResultUsername</t>
+  </si>
+  <si>
+    <t>(//div[contains(text(),'Admin')])</t>
   </si>
 </sst>
 </file>
@@ -150,7 +168,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -323,35 +341,35 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
@@ -373,6 +391,17 @@
         <v>0</v>
       </c>
       <c r="C20" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Search user using user role
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="42">
   <si>
     <t/>
   </si>
@@ -124,6 +124,21 @@
   </si>
   <si>
     <t>(//div[contains(text(),'Admin')])</t>
+  </si>
+  <si>
+    <t>UM_searchUserRole</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/div[2]/div[2]/div/div[1]/div[2]/form/div[1]/div/div[2]/div/div[2]/div/div</t>
+  </si>
+  <si>
+    <t>UM_selectUserRole</t>
+  </si>
+  <si>
+    <t>UM_searchResultUserRole</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/div[2]/div[2]/div/div[2]/div[3]/div/div[2]/div[1]/div/div[3]/div</t>
   </si>
 </sst>
 </file>
@@ -374,35 +389,35 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Search user using employee name
</commit_message>
<xml_diff>
--- a/data/locatorsRepository.xlsx
+++ b/data/locatorsRepository.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="46">
   <si>
     <t/>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>//*[@id="app"]/div[1]/div[2]/div[2]/div/div[2]/div[3]/div/div[2]/div[1]/div/div[3]/div</t>
+  </si>
+  <si>
+    <t>UM_searchEmployeeName</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/div[2]/div[2]/div/div[1]/div[2]/form/div[1]/div/div[3]/div/div[2]/div/div/input</t>
+  </si>
+  <si>
+    <t>UM_searchResultEmployeeName</t>
+  </si>
+  <si>
+    <t>//*[@id="app"]/div[1]/div[2]/div[2]/div/div[2]/div[3]/div/div[2]/div/div/div[4]/div</t>
   </si>
 </sst>
 </file>
@@ -183,7 +195,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -418,6 +430,116 @@
       </c>
       <c r="C21" t="s" s="0">
         <v>6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>